<commit_message>
add user input for charge number and date
</commit_message>
<xml_diff>
--- a/Total_hours.xlsx
+++ b/Total_hours.xlsx
@@ -131,26 +131,23 @@
   <commentList>
     <comment ref="D4" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">Jose (45)
+        <t>Jose (45)
 Philip (36)
-Dillon (45)
-</t>
+Dillon (45)</t>
       </text>
     </comment>
     <comment ref="D5" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">Philip (45)
+        <t>Philip (45)
 Dillon (36)
-Jose (36)
-</t>
+Jose (36)</t>
       </text>
     </comment>
     <comment ref="D6" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">Dillon (36)
+        <t>Dillon (36)
 Jose (36)
-Philip (36)
-</t>
+Philip (36)</t>
       </text>
     </comment>
   </commentList>

</xml_diff>